<commit_message>
Version 1.2: Add build AlarmList file func
</commit_message>
<xml_diff>
--- a/Conf/Config.xlsx
+++ b/Conf/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="648" windowWidth="14808" windowHeight="7476" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="768" windowWidth="14808" windowHeight="7356" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Conveyor" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="TestDataTemplate" sheetId="3" r:id="rId3"/>
     <sheet name="XmlTemplate" sheetId="4" r:id="rId4"/>
     <sheet name="L1AlarmDataTemple" sheetId="5" r:id="rId5"/>
+    <sheet name="OPCDataTemplate" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="146">
   <si>
     <t>System</t>
   </si>
@@ -470,6 +471,24 @@
   </si>
   <si>
     <t>Powerbox_4_Single2</t>
+  </si>
+  <si>
+    <t>{0}_{1}_{2}_{3}_SIGNAL_{4}</t>
+  </si>
+  <si>
+    <t>{0}_{1}_{2}_{3}_CM</t>
+  </si>
+  <si>
+    <t>{0}_{1}_{2}_{3}_Hour</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC01_TL35_BC045_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC07_EB03_BC019_CM</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC07_EB03_BC019_Hour</t>
   </si>
 </sst>
 </file>
@@ -814,7 +833,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,7 +978,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B16" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1233,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -1615,4 +1634,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>